<commit_message>
Ez már a második módosítés.
</commit_message>
<xml_diff>
--- a/valami.xlsx
+++ b/valami.xlsx
@@ -53,7 +53,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +114,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +149,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -333,10 +333,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>